<commit_message>
TaskWatclist tc19 - tc20_1
Signed-off-by: Akul Bhutani <navatariptesting@gmail.com>
</commit_message>
<xml_diff>
--- a/TaskWatchlist.xlsx
+++ b/TaskWatchlist.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="EntityorAccount" sheetId="5" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="131" uniqueCount="98">
   <si>
     <t>Variable_Name</t>
   </si>
@@ -317,6 +317,12 @@
   </si>
   <si>
     <t>CR Task 1</t>
+  </si>
+  <si>
+    <t>TWTask9</t>
+  </si>
+  <si>
+    <t>Update Label Task 1</t>
   </si>
 </sst>
 </file>
@@ -432,10 +438,10 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="2" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink 2" xfId="1"/>
@@ -940,7 +946,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AML18"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
@@ -1056,7 +1062,7 @@
       <c r="D2" t="s">
         <v>42</v>
       </c>
-      <c r="Y2" s="11" t="s">
+      <c r="Y2" s="12" t="s">
         <v>24</v>
       </c>
     </row>
@@ -1073,7 +1079,7 @@
       <c r="D3" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="Y3" s="11"/>
+      <c r="Y3" s="12"/>
     </row>
     <row r="4" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
@@ -1088,7 +1094,7 @@
       <c r="D4" s="2" t="s">
         <v>42</v>
       </c>
-      <c r="Y4" s="11"/>
+      <c r="Y4" s="12"/>
     </row>
     <row r="5" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A5" s="5" t="s">
@@ -1103,7 +1109,7 @@
       <c r="D5" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="Y5" s="11"/>
+      <c r="Y5" s="12"/>
     </row>
     <row r="6" spans="1:25" x14ac:dyDescent="0.25">
       <c r="M6" s="2" t="s">
@@ -1127,25 +1133,25 @@
       <c r="X6" s="2">
         <v>554477331</v>
       </c>
-      <c r="Y6" s="11"/>
+      <c r="Y6" s="12"/>
     </row>
     <row r="10" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B10" s="5"/>
-      <c r="Y10" s="11" t="s">
+      <c r="Y10" s="12" t="s">
         <v>24</v>
       </c>
     </row>
     <row r="11" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B11" s="5"/>
-      <c r="Y11" s="11"/>
+      <c r="Y11" s="12"/>
     </row>
     <row r="12" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B12" s="5"/>
-      <c r="Y12" s="11"/>
+      <c r="Y12" s="12"/>
     </row>
     <row r="13" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B13" s="5"/>
-      <c r="Y13" s="11"/>
+      <c r="Y13" s="12"/>
     </row>
     <row r="14" spans="1:25" x14ac:dyDescent="0.25">
       <c r="M14" s="2" t="s">
@@ -1169,7 +1175,7 @@
       <c r="X14" s="2">
         <v>554477331</v>
       </c>
-      <c r="Y14" s="11"/>
+      <c r="Y14" s="12"/>
     </row>
     <row r="15" spans="1:25" x14ac:dyDescent="0.25">
       <c r="B15" s="5"/>
@@ -1324,10 +1330,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K9"/>
+  <dimension ref="A1:K11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C9" sqref="C9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1457,12 +1463,23 @@
       </c>
     </row>
     <row r="9" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="11" t="s">
         <v>95</v>
       </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A10" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C10" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A11" s="11"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>